<commit_message>
Corretto file “report-checklist.xlsx” in modo che il "subject application vendor" indicato coincida esattamente con quello indicato nel path della cartella in cui i file sono inseriti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA/LeoLab/5.02023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA/LeoLab/5.02023/report-checklist.xlsx
@@ -4567,9 +4567,6 @@
     <t>subject_application_id:  LeoLab</t>
   </si>
   <si>
-    <t>subject_application_vendor: GIOTTO INFORMATICA S.a.s.</t>
-  </si>
-  <si>
     <t>subject_application_version: 5.0/2023</t>
   </si>
   <si>
@@ -4691,6 +4688,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.cfea25fb1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>subject_application_vendor: GIOTTO INFORMATICA</t>
   </si>
 </sst>
 </file>
@@ -5907,7 +5907,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8075,10 +8075,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -8121,7 +8121,7 @@
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="39" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D2" s="38"/>
       <c r="F2" s="12"/>
@@ -8169,7 +8169,7 @@
       <c r="A4" s="42"/>
       <c r="B4" s="43"/>
       <c r="C4" s="46" t="s">
-        <v>850</v>
+        <v>891</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="4"/>
@@ -8193,7 +8193,7 @@
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="46" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D5" s="38"/>
       <c r="F5" s="12"/>
@@ -8351,13 +8351,13 @@
         <v>45206</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>139</v>
@@ -8397,13 +8397,13 @@
         <v>45206</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>139</v>
@@ -8443,13 +8443,13 @@
         <v>45206</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>139</v>
@@ -8489,13 +8489,13 @@
         <v>45206</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>139</v>
@@ -8535,13 +8535,13 @@
         <v>45206</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>139</v>
@@ -9261,13 +9261,13 @@
         <v>45177</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J35" s="25" t="s">
         <v>139</v>
@@ -9280,13 +9280,13 @@
         <v>139</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="O35" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P35" s="25" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -9553,13 +9553,13 @@
         <v>45177</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>139</v>
@@ -9572,13 +9572,13 @@
         <v>139</v>
       </c>
       <c r="N43" s="25" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="O43" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P43" s="25" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
@@ -9858,13 +9858,13 @@
         <v>139</v>
       </c>
       <c r="N51" s="25" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="O51" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P51" s="25" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
@@ -10149,7 +10149,7 @@
         <v>848</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
@@ -10187,7 +10187,7 @@
         <v>848</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -10225,7 +10225,7 @@
         <v>848</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -10263,7 +10263,7 @@
         <v>848</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
@@ -10301,7 +10301,7 @@
         <v>848</v>
       </c>
       <c r="K63" s="34" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
@@ -10339,7 +10339,7 @@
         <v>848</v>
       </c>
       <c r="K64" s="34" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="L64" s="25"/>
       <c r="M64" s="25"/>
@@ -10377,7 +10377,7 @@
         <v>848</v>
       </c>
       <c r="K65" s="34" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L65" s="25"/>
       <c r="M65" s="25"/>
@@ -10415,7 +10415,7 @@
         <v>848</v>
       </c>
       <c r="K66" s="34" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L66" s="25"/>
       <c r="M66" s="25"/>
@@ -10453,7 +10453,7 @@
         <v>848</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -10491,7 +10491,7 @@
         <v>848</v>
       </c>
       <c r="K68" s="34" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="L68" s="25"/>
       <c r="M68" s="25"/>
@@ -10529,7 +10529,7 @@
         <v>848</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="L69" s="25"/>
       <c r="M69" s="25"/>
@@ -14919,7 +14919,7 @@
         <v>848</v>
       </c>
       <c r="K198" s="25" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -20937,13 +20937,13 @@
         <v>45206</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H375" s="24" t="s">
+        <v>884</v>
+      </c>
+      <c r="I375" s="24" t="s">
         <v>885</v>
-      </c>
-      <c r="I375" s="24" t="s">
-        <v>886</v>
       </c>
       <c r="J375" s="25" t="s">
         <v>139</v>
@@ -21225,7 +21225,7 @@
         <v>848</v>
       </c>
       <c r="K383" s="25" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>

</xml_diff>